<commit_message>
update column name in excel file
</commit_message>
<xml_diff>
--- a/spec/fixtures/requirements/requirements_test_kit_requirements.xlsx
+++ b/spec/fixtures/requirements/requirements_test_kit_requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smacvicar/code/inferno/spec/fixtures/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9801514-88C2-5B40-AAE0-7875A2EC0433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A3D49C-884C-4340-B47D-E198DD93010C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67460" windowHeight="21100" firstSheet="1" activeTab="2" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="67460" windowHeight="21100" firstSheet="1" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1214,9 +1214,6 @@
     <t>Conformance*</t>
   </si>
   <si>
-    <t>Actor*</t>
-  </si>
-  <si>
     <t>Sub-Requirement(s)</t>
   </si>
   <si>
@@ -1644,6 +1641,9 @@
   </si>
   <si>
     <t>requirement_set_id</t>
+  </si>
+  <si>
+    <t>Actors*</t>
   </si>
 </sst>
 </file>
@@ -2549,11 +2549,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
   <dimension ref="A1:AE141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2596,52 +2596,52 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="J1" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="K1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="L1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="M1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="T1" s="15" t="s">
-        <v>27</v>
       </c>
       <c r="Y1" s="6"/>
     </row>
@@ -2650,23 +2650,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="7" t="b">
         <v>1</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
@@ -2694,16 +2694,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="D3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="G3" s="7" t="b">
         <v>0</v>
@@ -2729,16 +2729,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="G4" s="7" t="b">
         <v>0</v>
@@ -2764,31 +2764,31 @@
         <v>12</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>41</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="7" t="b">
         <v>1</v>
       </c>
       <c r="H5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="K5" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="L5" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="L5" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="M5" s="9" t="str" cm="1">
         <f t="array" ref="M5">PAGE_NAME(B5)</f>
@@ -2804,22 +2804,22 @@
         <v>16</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="7" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M6" s="9" t="str" cm="1">
         <f t="array" ref="M6">PAGE_NAME(B6)</f>
@@ -2835,22 +2835,22 @@
         <v>21</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M7" s="9" t="str" cm="1">
         <f t="array" ref="M7">PAGE_NAME(B7)</f>
@@ -2867,19 +2867,19 @@
         <v>33</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="G8" s="7" t="b">
         <v>0</v>
@@ -2898,19 +2898,19 @@
         <v>34</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="G9" s="7" t="b">
         <v>0</v>
@@ -2929,32 +2929,32 @@
         <v>96</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="7" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I10" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="L10" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="L10" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="M10" s="9" t="str" cm="1">
         <f t="array" ref="M10">PAGE_NAME(B10)</f>
@@ -2970,22 +2970,22 @@
         <v>97</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="G11" s="7" t="b">
         <v>1</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M11" s="9" t="str" cm="1">
         <f t="array" ref="M11">PAGE_NAME(B11)</f>
@@ -3001,16 +3001,16 @@
         <v>98</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="G12" s="7" t="b">
         <v>0</v>
@@ -4375,7 +4375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C323F474-BE25-4449-9222-E1A46A1843B5}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -4387,7 +4387,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="44"/>
     </row>
@@ -4397,72 +4397,72 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>62</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="37"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="38"/>
     </row>
@@ -4494,19 +4494,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>75</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4514,13 +4514,13 @@
         <v>0.1</v>
       </c>
       <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
         <v>77</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -4540,67 +4540,67 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>81</v>
-      </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -4609,6 +4609,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC335ED7BB179244BF94A0DFE64544DC" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a0f66abe5d2a0564332877ab55d3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebd8b74-b9de-41b2-9247-c010c4973c2b" xmlns:ns3="b7009bbd-f938-489b-a530-f05273710fff" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec7ca2ee893ff8a0f61d4046c6461645" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
@@ -4862,19 +4875,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4885,6 +4885,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12FB330C-B068-4EE3-928A-A72A297ABA91}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4904,24 +4922,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
FI-4173: Allow requirements to have multiple actors (#701)
* allow multiple actors

* rename actor field to actors

* update column name in excel file

* don't load deprecated requirements
</commit_message>
<xml_diff>
--- a/spec/fixtures/requirements/requirements_test_kit_requirements.xlsx
+++ b/spec/fixtures/requirements/requirements_test_kit_requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smacvicar/code/inferno/spec/fixtures/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9801514-88C2-5B40-AAE0-7875A2EC0433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A3D49C-884C-4340-B47D-E198DD93010C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67460" windowHeight="21100" firstSheet="1" activeTab="2" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="67460" windowHeight="21100" firstSheet="1" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1214,9 +1214,6 @@
     <t>Conformance*</t>
   </si>
   <si>
-    <t>Actor*</t>
-  </si>
-  <si>
     <t>Sub-Requirement(s)</t>
   </si>
   <si>
@@ -1644,6 +1641,9 @@
   </si>
   <si>
     <t>requirement_set_id</t>
+  </si>
+  <si>
+    <t>Actors*</t>
   </si>
 </sst>
 </file>
@@ -2549,11 +2549,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
   <dimension ref="A1:AE141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2596,52 +2596,52 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="J1" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="K1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="L1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="M1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="T1" s="15" t="s">
-        <v>27</v>
       </c>
       <c r="Y1" s="6"/>
     </row>
@@ -2650,23 +2650,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="7" t="b">
         <v>1</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
@@ -2694,16 +2694,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="D3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="G3" s="7" t="b">
         <v>0</v>
@@ -2729,16 +2729,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="G4" s="7" t="b">
         <v>0</v>
@@ -2764,31 +2764,31 @@
         <v>12</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>41</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="7" t="b">
         <v>1</v>
       </c>
       <c r="H5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="K5" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="L5" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="L5" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="M5" s="9" t="str" cm="1">
         <f t="array" ref="M5">PAGE_NAME(B5)</f>
@@ -2804,22 +2804,22 @@
         <v>16</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="7" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M6" s="9" t="str" cm="1">
         <f t="array" ref="M6">PAGE_NAME(B6)</f>
@@ -2835,22 +2835,22 @@
         <v>21</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M7" s="9" t="str" cm="1">
         <f t="array" ref="M7">PAGE_NAME(B7)</f>
@@ -2867,19 +2867,19 @@
         <v>33</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="G8" s="7" t="b">
         <v>0</v>
@@ -2898,19 +2898,19 @@
         <v>34</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="G9" s="7" t="b">
         <v>0</v>
@@ -2929,32 +2929,32 @@
         <v>96</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="7" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I10" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="L10" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="L10" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="M10" s="9" t="str" cm="1">
         <f t="array" ref="M10">PAGE_NAME(B10)</f>
@@ -2970,22 +2970,22 @@
         <v>97</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="G11" s="7" t="b">
         <v>1</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M11" s="9" t="str" cm="1">
         <f t="array" ref="M11">PAGE_NAME(B11)</f>
@@ -3001,16 +3001,16 @@
         <v>98</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="G12" s="7" t="b">
         <v>0</v>
@@ -4375,7 +4375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C323F474-BE25-4449-9222-E1A46A1843B5}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -4387,7 +4387,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="44"/>
     </row>
@@ -4397,72 +4397,72 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>62</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="37"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="38"/>
     </row>
@@ -4494,19 +4494,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>75</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4514,13 +4514,13 @@
         <v>0.1</v>
       </c>
       <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
         <v>77</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -4540,67 +4540,67 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>81</v>
-      </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -4609,6 +4609,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC335ED7BB179244BF94A0DFE64544DC" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a0f66abe5d2a0564332877ab55d3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebd8b74-b9de-41b2-9247-c010c4973c2b" xmlns:ns3="b7009bbd-f938-489b-a530-f05273710fff" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec7ca2ee893ff8a0f61d4046c6461645" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
@@ -4862,19 +4875,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4885,6 +4885,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12FB330C-B068-4EE3-928A-A72A297ABA91}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4904,24 +4922,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
   <ds:schemaRefs>

</xml_diff>